<commit_message>
Resolved css issue of data table on listing page.
</commit_message>
<xml_diff>
--- a/docs/DB_Design.xlsx
+++ b/docs/DB_Design.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>Sr No.</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>effective date</t>
+  </si>
+  <si>
+    <t>valid_ip_addresses</t>
   </si>
   <si>
     <t>terms and conditions</t>
@@ -132,11 +135,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -158,6 +162,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -202,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,6 +224,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,10 +248,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -453,7 +469,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -504,11 +520,16 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C51" s="0" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>